<commit_message>
eirini updated catalog with 98% coverage
</commit_message>
<xml_diff>
--- a/nmadb/479688.xlsx
+++ b/nmadb/479688.xlsx
@@ -8,7 +8,7 @@
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
-    <sheet name="Feuil2" sheetId="2" r:id="rId2"/>
+    <sheet name="sensitivity analysis" sheetId="2" r:id="rId2"/>
     <sheet name="Feuil3" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="124519"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="29">
   <si>
     <t>study year</t>
   </si>
@@ -24,25 +24,16 @@
     <t>study name</t>
   </si>
   <si>
-    <t>Study id</t>
-  </si>
-  <si>
     <t>t1</t>
   </si>
   <si>
     <t>t2</t>
   </si>
   <si>
-    <t>RR</t>
-  </si>
-  <si>
     <t>CIL</t>
   </si>
   <si>
     <t>CIH</t>
-  </si>
-  <si>
-    <t>SE</t>
   </si>
   <si>
     <t>Harm</t>
@@ -120,6 +111,18 @@
   </si>
   <si>
     <t xml:space="preserve">GREACE </t>
+  </si>
+  <si>
+    <t>effect=HR</t>
+  </si>
+  <si>
+    <t>effect</t>
+  </si>
+  <si>
+    <t>id</t>
+  </si>
+  <si>
+    <t>se</t>
   </si>
 </sst>
 </file>
@@ -760,7 +763,7 @@
     <xf numFmtId="0" fontId="21" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="27">
+  <cellXfs count="29">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1"/>
@@ -806,6 +809,8 @@
     <xf numFmtId="0" fontId="13" fillId="34" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="2" fontId="12" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyAlignment="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="43">
     <cellStyle name="20% - Accent1" xfId="2"/>
@@ -826,12 +831,12 @@
     <cellStyle name="60% - Accent4" xfId="17"/>
     <cellStyle name="60% - Accent5" xfId="18"/>
     <cellStyle name="60% - Accent6" xfId="19"/>
-    <cellStyle name="Accent1 2" xfId="20" customBuiltin="1"/>
-    <cellStyle name="Accent2 2" xfId="21" customBuiltin="1"/>
-    <cellStyle name="Accent3 2" xfId="22" customBuiltin="1"/>
-    <cellStyle name="Accent4 2" xfId="23" customBuiltin="1"/>
-    <cellStyle name="Accent5 2" xfId="24" customBuiltin="1"/>
-    <cellStyle name="Accent6 2" xfId="25" customBuiltin="1"/>
+    <cellStyle name="Accent1 2" xfId="20"/>
+    <cellStyle name="Accent2 2" xfId="21"/>
+    <cellStyle name="Accent3 2" xfId="22"/>
+    <cellStyle name="Accent4 2" xfId="23"/>
+    <cellStyle name="Accent5 2" xfId="24"/>
+    <cellStyle name="Accent6 2" xfId="25"/>
     <cellStyle name="Bad" xfId="26"/>
     <cellStyle name="Calculation" xfId="27"/>
     <cellStyle name="Check Cell" xfId="28"/>
@@ -849,7 +854,7 @@
     <cellStyle name="Note" xfId="38"/>
     <cellStyle name="Output" xfId="39"/>
     <cellStyle name="Title" xfId="40"/>
-    <cellStyle name="Total 2" xfId="41" customBuiltin="1"/>
+    <cellStyle name="Total 2" xfId="41"/>
     <cellStyle name="Warning Text" xfId="42"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1142,13 +1147,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:O13"/>
+  <dimension ref="A1:O10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C19" sqref="C19"/>
+      <selection activeCell="A11" sqref="A11:XFD13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <cols>
+    <col min="9" max="9" width="11.42578125" style="28"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:15" ht="15.75" thickBot="1">
       <c r="A1" s="7" t="s">
@@ -1158,32 +1166,32 @@
         <v>1</v>
       </c>
       <c r="C1" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="D1" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="7" t="s">
+      <c r="E1" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="7" t="s">
+      <c r="F1" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="G1" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="8" t="s">
+      <c r="H1" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="8" t="s">
-        <v>6</v>
-      </c>
-      <c r="H1" s="8" t="s">
-        <v>7</v>
-      </c>
       <c r="I1" s="8" t="s">
-        <v>8</v>
+        <v>28</v>
       </c>
       <c r="J1" s="8"/>
       <c r="K1" s="4" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="L1" s="2" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="M1" s="1"/>
       <c r="N1" s="11"/>
@@ -1194,7 +1202,7 @@
         <v>1994</v>
       </c>
       <c r="B2" s="10" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="C2" s="5">
         <v>1</v>
@@ -1214,17 +1222,20 @@
       <c r="H2" s="5">
         <v>0.77</v>
       </c>
-      <c r="I2" s="1"/>
+      <c r="I2" s="27">
+        <f>(H2-G2)/(1.96^2)</f>
+        <v>3.9046230737192843E-2</v>
+      </c>
       <c r="J2" s="1"/>
       <c r="K2" s="1"/>
       <c r="L2" s="15" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="M2" s="16">
         <v>1</v>
       </c>
       <c r="N2" s="17" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="O2" s="1"/>
     </row>
@@ -1233,7 +1244,7 @@
         <v>2002</v>
       </c>
       <c r="B3" s="10" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="C3" s="5">
         <v>2</v>
@@ -1253,7 +1264,10 @@
       <c r="H3" s="5">
         <v>0.8</v>
       </c>
-      <c r="I3" s="1"/>
+      <c r="I3" s="27">
+        <f>(H3-G3)/(1.96^2)</f>
+        <v>3.1236984589754272E-2</v>
+      </c>
       <c r="J3" s="1"/>
       <c r="K3" s="1"/>
       <c r="L3" s="18"/>
@@ -1261,7 +1275,7 @@
         <v>2</v>
       </c>
       <c r="N3" s="19" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="O3" s="1"/>
     </row>
@@ -1270,7 +1284,7 @@
         <v>1996</v>
       </c>
       <c r="B4" s="10" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="C4" s="5">
         <v>3</v>
@@ -1290,7 +1304,10 @@
       <c r="H4" s="5">
         <v>0.91</v>
       </c>
-      <c r="I4" s="1"/>
+      <c r="I4" s="27">
+        <f>(H4-G4)/(1.96^2)</f>
+        <v>6.7680133277800925E-2</v>
+      </c>
       <c r="J4" s="1"/>
       <c r="K4" s="1"/>
       <c r="L4" s="18"/>
@@ -1298,7 +1315,7 @@
         <v>3</v>
       </c>
       <c r="N4" s="19" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="O4" s="1"/>
     </row>
@@ -1307,7 +1324,7 @@
         <v>1998</v>
       </c>
       <c r="B5" s="10" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="C5" s="5">
         <v>4</v>
@@ -1327,7 +1344,10 @@
       <c r="H5" s="5">
         <v>0.86</v>
       </c>
-      <c r="I5" s="1"/>
+      <c r="I5" s="27">
+        <f>(H5-G5)/(1.96^2)</f>
+        <v>4.1649312786339036E-2</v>
+      </c>
       <c r="J5" s="1"/>
       <c r="K5" s="1"/>
       <c r="L5" s="20"/>
@@ -1335,7 +1355,7 @@
         <v>4</v>
       </c>
       <c r="N5" s="22" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="O5" s="1"/>
     </row>
@@ -1344,7 +1364,7 @@
         <v>2002</v>
       </c>
       <c r="B6" s="10" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="C6" s="5">
         <v>5</v>
@@ -1364,7 +1384,10 @@
       <c r="H6" s="5">
         <v>0.96</v>
       </c>
-      <c r="I6" s="1"/>
+      <c r="I6" s="27">
+        <f>(H6-G6)/(1.96^2)</f>
+        <v>6.5077051228654731E-2</v>
+      </c>
       <c r="J6" s="1"/>
       <c r="K6" s="1"/>
       <c r="L6" s="12"/>
@@ -1377,7 +1400,7 @@
         <v>1995</v>
       </c>
       <c r="B7" s="10" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="C7" s="5">
         <v>6</v>
@@ -1397,11 +1420,14 @@
       <c r="H7" s="5">
         <v>0.84</v>
       </c>
-      <c r="I7" s="1"/>
+      <c r="I7" s="27">
+        <f>(H7-G7)/(1.96^2)</f>
+        <v>6.7680133277800925E-2</v>
+      </c>
       <c r="J7" s="1"/>
       <c r="K7" s="1"/>
       <c r="L7" s="26" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="M7" s="26"/>
       <c r="N7" s="26"/>
@@ -1412,7 +1438,7 @@
         <v>2003</v>
       </c>
       <c r="B8" s="10" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="C8" s="5">
         <v>7</v>
@@ -1432,7 +1458,10 @@
       <c r="H8" s="5">
         <v>0.81</v>
       </c>
-      <c r="I8" s="1"/>
+      <c r="I8" s="27">
+        <f>(H8-G8)/(1.96^2)</f>
+        <v>8.5901707621824266E-2</v>
+      </c>
       <c r="J8" s="1"/>
       <c r="K8" s="1"/>
       <c r="L8" s="26"/>
@@ -1445,7 +1474,7 @@
         <v>2004</v>
       </c>
       <c r="B9" s="10" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="C9" s="5">
         <v>8</v>
@@ -1465,7 +1494,10 @@
       <c r="H9" s="5">
         <v>0.81</v>
       </c>
-      <c r="I9" s="1"/>
+      <c r="I9" s="27">
+        <f>(H9-G9)/(1.96^2)</f>
+        <v>0.11974177426072473</v>
+      </c>
       <c r="J9" s="1"/>
       <c r="K9" s="1"/>
       <c r="L9" s="26"/>
@@ -1482,98 +1514,13 @@
       <c r="F10" s="1"/>
       <c r="G10" s="1"/>
       <c r="H10" s="1"/>
-      <c r="I10" s="1"/>
+      <c r="I10" s="27"/>
       <c r="J10" s="1"/>
       <c r="K10" s="1"/>
       <c r="L10" s="26"/>
       <c r="M10" s="26"/>
       <c r="N10" s="26"/>
       <c r="O10" s="26"/>
-    </row>
-    <row r="11" spans="1:15">
-      <c r="A11" s="25" t="s">
-        <v>25</v>
-      </c>
-      <c r="B11" s="23"/>
-      <c r="C11" s="24"/>
-      <c r="D11" s="24"/>
-      <c r="E11" s="24"/>
-      <c r="F11" s="24"/>
-      <c r="G11" s="24"/>
-      <c r="H11" s="24"/>
-      <c r="I11" s="1"/>
-      <c r="J11" s="1"/>
-      <c r="K11" s="1"/>
-      <c r="L11" s="4"/>
-      <c r="M11" s="4"/>
-      <c r="N11" s="1"/>
-      <c r="O11" s="1"/>
-    </row>
-    <row r="12" spans="1:15">
-      <c r="A12" s="6">
-        <v>2002</v>
-      </c>
-      <c r="B12" s="10" t="s">
-        <v>26</v>
-      </c>
-      <c r="C12" s="5">
-        <v>9</v>
-      </c>
-      <c r="D12" s="5">
-        <v>1</v>
-      </c>
-      <c r="E12" s="5">
-        <v>3</v>
-      </c>
-      <c r="F12" s="5">
-        <v>0.91</v>
-      </c>
-      <c r="G12" s="5">
-        <v>0.79</v>
-      </c>
-      <c r="H12" s="5">
-        <v>1.03</v>
-      </c>
-      <c r="I12" s="1"/>
-      <c r="J12" s="1"/>
-      <c r="K12" s="1"/>
-      <c r="L12" s="1"/>
-      <c r="M12" s="1"/>
-      <c r="N12" s="1"/>
-      <c r="O12" s="1"/>
-    </row>
-    <row r="13" spans="1:15">
-      <c r="A13" s="6">
-        <v>2002</v>
-      </c>
-      <c r="B13" s="10" t="s">
-        <v>27</v>
-      </c>
-      <c r="C13" s="5">
-        <v>10</v>
-      </c>
-      <c r="D13" s="5">
-        <v>1</v>
-      </c>
-      <c r="E13" s="5">
-        <v>4</v>
-      </c>
-      <c r="F13" s="5">
-        <v>0.46</v>
-      </c>
-      <c r="G13" s="5">
-        <v>0.32</v>
-      </c>
-      <c r="H13" s="5">
-        <v>0.66</v>
-      </c>
-      <c r="I13" s="1"/>
-      <c r="J13" s="1"/>
-      <c r="K13" s="1"/>
-      <c r="L13" s="1"/>
-      <c r="M13" s="1"/>
-      <c r="N13" s="1"/>
-      <c r="O13" s="1"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -1585,12 +1532,108 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1"/>
+  <dimension ref="A1:O3"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D26" sqref="D26"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
-  <sheetData/>
+  <sheetData>
+    <row r="1" spans="1:15">
+      <c r="A1" s="25" t="s">
+        <v>22</v>
+      </c>
+      <c r="B1" s="23"/>
+      <c r="C1" s="24"/>
+      <c r="D1" s="24"/>
+      <c r="E1" s="24"/>
+      <c r="F1" s="24"/>
+      <c r="G1" s="24"/>
+      <c r="H1" s="24"/>
+      <c r="I1" s="27"/>
+      <c r="J1" s="1"/>
+      <c r="K1" s="1"/>
+      <c r="L1" s="4"/>
+      <c r="M1" s="4"/>
+      <c r="N1" s="1"/>
+      <c r="O1" s="1"/>
+    </row>
+    <row r="2" spans="1:15">
+      <c r="A2" s="6">
+        <v>2002</v>
+      </c>
+      <c r="B2" s="10" t="s">
+        <v>23</v>
+      </c>
+      <c r="C2" s="5">
+        <v>9</v>
+      </c>
+      <c r="D2" s="5">
+        <v>1</v>
+      </c>
+      <c r="E2" s="5">
+        <v>3</v>
+      </c>
+      <c r="F2" s="5">
+        <v>0.91</v>
+      </c>
+      <c r="G2" s="5">
+        <v>0.79</v>
+      </c>
+      <c r="H2" s="5">
+        <v>1.03</v>
+      </c>
+      <c r="I2" s="27">
+        <f>(H2-G2)/(1.96^2)</f>
+        <v>6.2473969179508544E-2</v>
+      </c>
+      <c r="J2" s="1"/>
+      <c r="K2" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="L2" s="1"/>
+      <c r="M2" s="1"/>
+      <c r="N2" s="1"/>
+      <c r="O2" s="1"/>
+    </row>
+    <row r="3" spans="1:15">
+      <c r="A3" s="6">
+        <v>2002</v>
+      </c>
+      <c r="B3" s="10" t="s">
+        <v>24</v>
+      </c>
+      <c r="C3" s="5">
+        <v>10</v>
+      </c>
+      <c r="D3" s="5">
+        <v>1</v>
+      </c>
+      <c r="E3" s="5">
+        <v>4</v>
+      </c>
+      <c r="F3" s="5">
+        <v>0.46</v>
+      </c>
+      <c r="G3" s="5">
+        <v>0.32</v>
+      </c>
+      <c r="H3" s="5">
+        <v>0.66</v>
+      </c>
+      <c r="I3" s="27">
+        <f>(H3-G3)/(1.96^2)</f>
+        <v>8.8504789670970446E-2</v>
+      </c>
+      <c r="J3" s="1"/>
+      <c r="K3" s="1"/>
+      <c r="L3" s="1"/>
+      <c r="M3" s="1"/>
+      <c r="N3" s="1"/>
+      <c r="O3" s="1"/>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>

</xml_diff>